<commit_message>
Sync all stuff before transfer
</commit_message>
<xml_diff>
--- a/docs/ItemTraits.xlsx
+++ b/docs/ItemTraits.xlsx
@@ -4,6 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <sheets>
     <sheet name="Лист1" r:id="rId1" sheetId="1" state="visible"/>
+    <sheet name="Лист2" r:id="rId2" sheetId="2" state="visible"/>
   </sheets>
   <definedNames/>
 </workbook>
@@ -159,10 +160,37 @@
     <t>Heaven</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>of Eddy's Son</t>
+    </r>
+  </si>
+  <si>
     <t>Magenta</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>of Thor'n</t>
+    </r>
+  </si>
+  <si>
     <t>Doom</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>of the Tesla</t>
+    </r>
   </si>
   <si>
     <t>Dragonskin</t>
@@ -211,6 +239,142 @@
       </rPr>
       <t>Nanofiber</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Dynamo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Solar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Atomic</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Cell-Powered</t>
+    </r>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>Max HP</t>
+  </si>
+  <si>
+    <t>armor of</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si/>
+  <si>
+    <t>Resist</t>
+  </si>
+  <si>
+    <t>ring of</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>Reduction</t>
+  </si>
+  <si>
+    <t>Extra Gold</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Greed</t>
+  </si>
+  <si>
+    <t>Treasure</t>
+  </si>
+  <si>
+    <t>Dmg Amp</t>
+  </si>
+  <si>
+    <t>Carnage</t>
+  </si>
+  <si>
+    <t>Violence</t>
+  </si>
+  <si>
+    <t>the Battlemaster</t>
+  </si>
+  <si>
+    <t>Dmg Reflect</t>
+  </si>
+  <si>
+    <t>Tenons</t>
+  </si>
+  <si>
+    <t>Ruffs</t>
+  </si>
+  <si>
+    <t>Vampirism</t>
+  </si>
+  <si>
+    <t>the Leech</t>
+  </si>
+  <si>
+    <t>HP Regen</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Reshape</t>
+  </si>
+  <si>
+    <t>HP on Kill</t>
+  </si>
+  <si>
+    <t>the Ghost</t>
+  </si>
+  <si>
+    <t>the Wraith</t>
   </si>
 </sst>
 </file>
@@ -237,11 +401,10 @@
       <sz val="12"/>
     </font>
     <font>
-      <name val="XO Thames"/>
-      <sz val="12"/>
+      <b val="true"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +414,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="92FF99" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE779" tint="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -266,11 +434,31 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="3" quotePrefix="false"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="4" quotePrefix="false"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="1" quotePrefix="false"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3" fontId="1" quotePrefix="false"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="4" quotePrefix="false"/>
+    <xf applyAlignment="true" borderId="0" fillId="0" fontId="0" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="4" quotePrefix="false">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="4" quotePrefix="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="4" quotePrefix="false">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -489,7 +677,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -745,13 +933,19 @@
       <c r="B22" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row outlineLevel="0" r="24">
@@ -759,7 +953,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row outlineLevel="0" r="25">
@@ -767,7 +964,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row outlineLevel="0" r="26">
@@ -775,7 +972,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row outlineLevel="0" r="27">
@@ -783,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row outlineLevel="0" r="28">
@@ -791,7 +988,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row outlineLevel="0" r="29">
@@ -799,7 +996,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row outlineLevel="0" r="30">
@@ -807,7 +1004,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row outlineLevel="0" r="31">
@@ -815,7 +1012,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row outlineLevel="0" r="32">
@@ -823,10 +1020,322 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.790000021457672" footer="0.19680555164814" header="0.19680555164814" left="0.790000021457672" right="0.790000021457672" top="0.790000021457672"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a15="http://schemas.microsoft.com/office/drawing/2012/main" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:co="http://ncloudtech.com" xmlns:co-ooxml="http://ncloudtech.com/ooxml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:x="urn:schemas-microsoft-com:office:excel" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="co co-ooxml w14 x14 w15">
+  <sheetPr>
+    <outlinePr summaryBelow="true" summaryRight="true"/>
+  </sheetPr>
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView showZeros="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" customHeight="false" defaultColWidth="10.7884703773945" defaultRowHeight="15" zeroHeight="false"/>
+  <cols>
+    <col bestFit="true" customWidth="true" max="1" min="1" outlineLevel="0" style="5" width="11.9969516254079"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" outlineLevel="0" width="9.10546039675898"/>
+    <col bestFit="true" customWidth="true" max="3" min="3" outlineLevel="0" width="10.1063612066759"/>
+    <col bestFit="true" customWidth="true" max="4" min="4" outlineLevel="0" width="9.57421041261831"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" outlineLevel="0" width="10.6416300717924"/>
+    <col bestFit="true" customWidth="true" max="6" min="6" outlineLevel="0" style="6" width="8.09728408770455"/>
+    <col bestFit="true" customWidth="true" max="7" min="7" outlineLevel="0" width="12.0572343325472"/>
+    <col bestFit="true" customWidth="true" max="8" min="8" outlineLevel="0" width="9.75194046297739"/>
+    <col bestFit="true" customWidth="true" max="10" min="9" outlineLevel="0" width="15.3083430899929"/>
+  </cols>
+  <sheetData>
+    <row customFormat="true" ht="15" outlineLevel="0" r="1" s="5">
+      <c r="A1" s="5" t="n"/>
+      <c r="B1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="8" t="n"/>
+      <c r="G1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="0" t="n"/>
+      <c r="G4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="n"/>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="0" t="n"/>
+      <c r="G5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="n"/>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="0" t="n"/>
+      <c r="G6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="0" t="n"/>
+      <c r="G7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="n"/>
+      <c r="G9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.590555548667908" footer="0.5" header="0.5" left="0.590555548667908" right="0.590555548667908" top="0.590555548667908"/>
+  <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297.1798mm" paperSize="9" paperWidth="210.0438mm" scale="100"/>
+</worksheet>
 </file>
</xml_diff>